<commit_message>
Edit 2016 09 05 03:37
</commit_message>
<xml_diff>
--- a/!List of all pieces.xlsx
+++ b/!List of all pieces.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Documents\bel-accueil\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2843,9 +2843,6 @@
     <t>splendens_ceptigera</t>
   </si>
   <si>
-    <t>stella_plendens</t>
-  </si>
-  <si>
     <t>sumer_is_icumen_in</t>
   </si>
   <si>
@@ -3072,6 +3069,9 @@
   </si>
   <si>
     <t>Takayama [鷹山]</t>
+  </si>
+  <si>
+    <t>stella_splendens</t>
   </si>
 </sst>
 </file>
@@ -3401,9 +3401,9 @@
   <dimension ref="A1:K239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomLeft" activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3482,7 +3482,7 @@
         <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3511,7 +3511,7 @@
         <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3540,7 +3540,7 @@
         <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3569,7 +3569,7 @@
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3598,7 +3598,7 @@
         <v>22</v>
       </c>
       <c r="J6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3627,7 +3627,7 @@
         <v>12</v>
       </c>
       <c r="J7" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3656,7 +3656,7 @@
         <v>31</v>
       </c>
       <c r="J8" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3711,7 +3711,7 @@
         <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3719,7 +3719,7 @@
         <v>741</v>
       </c>
       <c r="B11" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C11" t="s">
         <v>650</v>
@@ -3740,7 +3740,7 @@
         <v>42</v>
       </c>
       <c r="J11" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K11" t="s">
         <v>704</v>
@@ -3772,7 +3772,7 @@
         <v>35</v>
       </c>
       <c r="J12" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3824,7 +3824,7 @@
         <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3879,7 +3879,7 @@
         <v>42</v>
       </c>
       <c r="J16" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3908,7 +3908,7 @@
         <v>42</v>
       </c>
       <c r="J17" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3916,7 +3916,7 @@
         <v>747</v>
       </c>
       <c r="B18" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C18" t="s">
         <v>650</v>
@@ -3937,7 +3937,7 @@
         <v>42</v>
       </c>
       <c r="J18" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K18" t="s">
         <v>704</v>
@@ -3969,7 +3969,7 @@
         <v>35</v>
       </c>
       <c r="J19" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3977,7 +3977,7 @@
         <v>749</v>
       </c>
       <c r="B20" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C20" t="s">
         <v>650</v>
@@ -3998,7 +3998,7 @@
         <v>42</v>
       </c>
       <c r="J20" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K20" t="s">
         <v>704</v>
@@ -4009,7 +4009,7 @@
         <v>750</v>
       </c>
       <c r="B21" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C21" t="s">
         <v>650</v>
@@ -4030,7 +4030,7 @@
         <v>42</v>
       </c>
       <c r="J21" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K21" t="s">
         <v>704</v>
@@ -4062,7 +4062,7 @@
         <v>12</v>
       </c>
       <c r="J22" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -4122,7 +4122,7 @@
         <v>756</v>
       </c>
       <c r="B25" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C25" t="s">
         <v>650</v>
@@ -4143,7 +4143,7 @@
         <v>42</v>
       </c>
       <c r="J25" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K25" t="s">
         <v>704</v>
@@ -4175,7 +4175,7 @@
         <v>31</v>
       </c>
       <c r="J26" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -4204,7 +4204,7 @@
         <v>12</v>
       </c>
       <c r="J27" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -4259,7 +4259,7 @@
         <v>7</v>
       </c>
       <c r="J29" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -4288,7 +4288,7 @@
         <v>22</v>
       </c>
       <c r="J30" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -4314,7 +4314,7 @@
         <v>22</v>
       </c>
       <c r="J31" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -4346,7 +4346,7 @@
         <v>22</v>
       </c>
       <c r="J32" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>42</v>
       </c>
       <c r="J34" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="K34" t="s">
         <v>705</v>
@@ -4453,7 +4453,7 @@
         <v>12</v>
       </c>
       <c r="J36" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -4482,7 +4482,7 @@
         <v>12</v>
       </c>
       <c r="J37" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -4508,7 +4508,7 @@
         <v>12</v>
       </c>
       <c r="J38" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -4516,7 +4516,7 @@
         <v>769</v>
       </c>
       <c r="B39" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="C39" t="s">
         <v>650</v>
@@ -4537,7 +4537,7 @@
         <v>42</v>
       </c>
       <c r="J39" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K39" t="s">
         <v>704</v>
@@ -4595,7 +4595,7 @@
         <v>12</v>
       </c>
       <c r="J41" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -4624,7 +4624,7 @@
         <v>12</v>
       </c>
       <c r="J42" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -4653,7 +4653,7 @@
         <v>12</v>
       </c>
       <c r="J43" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -4682,7 +4682,7 @@
         <v>12</v>
       </c>
       <c r="J44" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -4809,7 +4809,7 @@
         <v>7</v>
       </c>
       <c r="J49" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -4838,7 +4838,7 @@
         <v>22</v>
       </c>
       <c r="J50" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -4867,7 +4867,7 @@
         <v>12</v>
       </c>
       <c r="J51" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -4899,7 +4899,7 @@
         <v>31</v>
       </c>
       <c r="J52" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -4925,7 +4925,7 @@
         <v>12</v>
       </c>
       <c r="J53" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -5003,7 +5003,7 @@
         <v>31</v>
       </c>
       <c r="J56" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -5081,7 +5081,7 @@
         <v>12</v>
       </c>
       <c r="J59" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -5110,7 +5110,7 @@
         <v>42</v>
       </c>
       <c r="J60" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -5168,7 +5168,7 @@
         <v>162</v>
       </c>
       <c r="J62" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -5226,7 +5226,7 @@
         <v>12</v>
       </c>
       <c r="J64" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -5278,7 +5278,7 @@
         <v>31</v>
       </c>
       <c r="J66" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -5307,7 +5307,7 @@
         <v>22</v>
       </c>
       <c r="J67" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -5359,7 +5359,7 @@
         <v>31</v>
       </c>
       <c r="J69" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -5411,7 +5411,7 @@
         <v>12</v>
       </c>
       <c r="J71" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -5463,7 +5463,7 @@
         <v>7</v>
       </c>
       <c r="J73" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -5471,7 +5471,7 @@
         <v>806</v>
       </c>
       <c r="B74" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C74" t="s">
         <v>650</v>
@@ -5492,7 +5492,7 @@
         <v>42</v>
       </c>
       <c r="J74" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K74" t="s">
         <v>704</v>
@@ -5521,7 +5521,7 @@
         <v>12</v>
       </c>
       <c r="J75" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -5550,7 +5550,7 @@
         <v>35</v>
       </c>
       <c r="J76" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -5579,7 +5579,7 @@
         <v>12</v>
       </c>
       <c r="J77" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -5608,7 +5608,7 @@
         <v>42</v>
       </c>
       <c r="J78" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -5692,7 +5692,7 @@
         <v>22</v>
       </c>
       <c r="J81" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -5724,7 +5724,7 @@
         <v>35</v>
       </c>
       <c r="J82" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -5804,7 +5804,7 @@
         <v>818</v>
       </c>
       <c r="B86" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C86" t="s">
         <v>650</v>
@@ -5825,7 +5825,7 @@
         <v>42</v>
       </c>
       <c r="J86" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K86" t="s">
         <v>704</v>
@@ -5854,7 +5854,7 @@
         <v>42</v>
       </c>
       <c r="J87" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="K87" t="s">
         <v>588</v>
@@ -5912,7 +5912,7 @@
         <v>31</v>
       </c>
       <c r="J89" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -5946,7 +5946,7 @@
         <v>823</v>
       </c>
       <c r="B91" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C91" t="s">
         <v>650</v>
@@ -5967,7 +5967,7 @@
         <v>42</v>
       </c>
       <c r="J91" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K91" t="s">
         <v>704</v>
@@ -5996,7 +5996,7 @@
         <v>42</v>
       </c>
       <c r="J92" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -6169,7 +6169,7 @@
         <v>31</v>
       </c>
       <c r="J99" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -6177,7 +6177,7 @@
         <v>832</v>
       </c>
       <c r="B100" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C100" t="s">
         <v>650</v>
@@ -6198,7 +6198,7 @@
         <v>42</v>
       </c>
       <c r="J100" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K100" t="s">
         <v>704</v>
@@ -6209,7 +6209,7 @@
         <v>833</v>
       </c>
       <c r="B101" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C101" t="s">
         <v>650</v>
@@ -6230,7 +6230,7 @@
         <v>42</v>
       </c>
       <c r="J101" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K101" t="s">
         <v>704</v>
@@ -6241,7 +6241,7 @@
         <v>834</v>
       </c>
       <c r="B102" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C102" t="s">
         <v>650</v>
@@ -6262,7 +6262,7 @@
         <v>42</v>
       </c>
       <c r="J102" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K102" t="s">
         <v>704</v>
@@ -6340,7 +6340,7 @@
         <v>57</v>
       </c>
       <c r="J105" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -6369,7 +6369,7 @@
         <v>22</v>
       </c>
       <c r="J106" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -6398,7 +6398,7 @@
         <v>42</v>
       </c>
       <c r="J107" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -6476,7 +6476,7 @@
         <v>7</v>
       </c>
       <c r="J110" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -6577,7 +6577,7 @@
         <v>12</v>
       </c>
       <c r="J114" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
@@ -6603,7 +6603,7 @@
         <v>35</v>
       </c>
       <c r="J115" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
@@ -6655,7 +6655,7 @@
         <v>12</v>
       </c>
       <c r="J117" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
@@ -6710,7 +6710,7 @@
         <v>35</v>
       </c>
       <c r="J119" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -6718,7 +6718,7 @@
         <v>852</v>
       </c>
       <c r="B120" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C120" t="s">
         <v>650</v>
@@ -6739,7 +6739,7 @@
         <v>42</v>
       </c>
       <c r="J120" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K120" t="s">
         <v>704</v>
@@ -6831,7 +6831,7 @@
         <v>856</v>
       </c>
       <c r="B124" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C124" t="s">
         <v>650</v>
@@ -6852,7 +6852,7 @@
         <v>42</v>
       </c>
       <c r="J124" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K124" t="s">
         <v>704</v>
@@ -6863,7 +6863,7 @@
         <v>857</v>
       </c>
       <c r="B125" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C125" t="s">
         <v>650</v>
@@ -6884,7 +6884,7 @@
         <v>42</v>
       </c>
       <c r="J125" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K125" t="s">
         <v>704</v>
@@ -6913,7 +6913,7 @@
         <v>12</v>
       </c>
       <c r="J126" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
@@ -6921,7 +6921,7 @@
         <v>859</v>
       </c>
       <c r="B127" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C127" t="s">
         <v>650</v>
@@ -6942,7 +6942,7 @@
         <v>42</v>
       </c>
       <c r="J127" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K127" t="s">
         <v>704</v>
@@ -6974,7 +6974,7 @@
         <v>12</v>
       </c>
       <c r="J128" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
@@ -7003,7 +7003,7 @@
         <v>12</v>
       </c>
       <c r="J129" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
@@ -7011,7 +7011,7 @@
         <v>862</v>
       </c>
       <c r="B130" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C130" t="s">
         <v>650</v>
@@ -7032,7 +7032,7 @@
         <v>42</v>
       </c>
       <c r="J130" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K130" t="s">
         <v>704</v>
@@ -7043,7 +7043,7 @@
         <v>863</v>
       </c>
       <c r="B131" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C131" t="s">
         <v>650</v>
@@ -7064,7 +7064,7 @@
         <v>42</v>
       </c>
       <c r="J131" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K131" t="s">
         <v>704</v>
@@ -7096,7 +7096,7 @@
         <v>35</v>
       </c>
       <c r="J132" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="K132" t="s">
         <v>703</v>
@@ -7107,7 +7107,7 @@
         <v>865</v>
       </c>
       <c r="B133" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C133" t="s">
         <v>650</v>
@@ -7128,7 +7128,7 @@
         <v>42</v>
       </c>
       <c r="J133" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K133" t="s">
         <v>704</v>
@@ -7238,7 +7238,7 @@
         <v>42</v>
       </c>
       <c r="J137" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
@@ -7267,7 +7267,7 @@
         <v>42</v>
       </c>
       <c r="J138" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
@@ -7322,7 +7322,7 @@
         <v>12</v>
       </c>
       <c r="J140" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
@@ -7400,7 +7400,7 @@
         <v>22</v>
       </c>
       <c r="J143" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
@@ -7429,7 +7429,7 @@
         <v>12</v>
       </c>
       <c r="J144" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="K144" t="s">
         <v>584</v>
@@ -7519,7 +7519,7 @@
         <v>31</v>
       </c>
       <c r="J147" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
@@ -7550,7 +7550,7 @@
         <v>881</v>
       </c>
       <c r="B149" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C149" t="s">
         <v>650</v>
@@ -7571,7 +7571,7 @@
         <v>42</v>
       </c>
       <c r="J149" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K149" t="s">
         <v>704</v>
@@ -7605,7 +7605,7 @@
         <v>883</v>
       </c>
       <c r="B151" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C151" t="s">
         <v>650</v>
@@ -7626,7 +7626,7 @@
         <v>42</v>
       </c>
       <c r="J151" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K151" t="s">
         <v>704</v>
@@ -7637,7 +7637,7 @@
         <v>884</v>
       </c>
       <c r="B152" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C152" t="s">
         <v>650</v>
@@ -7658,7 +7658,7 @@
         <v>42</v>
       </c>
       <c r="J152" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K152" t="s">
         <v>704</v>
@@ -7736,7 +7736,7 @@
         <v>12</v>
       </c>
       <c r="J155" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="K155" t="s">
         <v>588</v>
@@ -7768,7 +7768,7 @@
         <v>22</v>
       </c>
       <c r="J156" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
@@ -7797,7 +7797,7 @@
         <v>7</v>
       </c>
       <c r="J157" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
@@ -7904,7 +7904,7 @@
         <v>42</v>
       </c>
       <c r="J161" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
@@ -7933,7 +7933,7 @@
         <v>50</v>
       </c>
       <c r="J162" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
@@ -7962,7 +7962,7 @@
         <v>12</v>
       </c>
       <c r="J163" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
@@ -7991,7 +7991,7 @@
         <v>12</v>
       </c>
       <c r="J164" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
@@ -8020,7 +8020,7 @@
         <v>12</v>
       </c>
       <c r="J165" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
@@ -8049,7 +8049,7 @@
         <v>12</v>
       </c>
       <c r="J166" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
@@ -8078,7 +8078,7 @@
         <v>42</v>
       </c>
       <c r="J167" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
@@ -8179,7 +8179,7 @@
         <v>12</v>
       </c>
       <c r="J171" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
@@ -8208,7 +8208,7 @@
         <v>31</v>
       </c>
       <c r="J172" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
@@ -8237,7 +8237,7 @@
         <v>35</v>
       </c>
       <c r="J173" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
@@ -8266,7 +8266,7 @@
         <v>162</v>
       </c>
       <c r="J174" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
@@ -8344,7 +8344,7 @@
         <v>42</v>
       </c>
       <c r="J177" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
@@ -8402,7 +8402,7 @@
         <v>12</v>
       </c>
       <c r="J179" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
@@ -8431,7 +8431,7 @@
         <v>12</v>
       </c>
       <c r="J180" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
@@ -8460,7 +8460,7 @@
         <v>12</v>
       </c>
       <c r="J181" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
@@ -8489,7 +8489,7 @@
         <v>12</v>
       </c>
       <c r="J182" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
@@ -8518,7 +8518,7 @@
         <v>12</v>
       </c>
       <c r="J183" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
@@ -8599,7 +8599,7 @@
         <v>22</v>
       </c>
       <c r="J186" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
@@ -8628,7 +8628,7 @@
         <v>42</v>
       </c>
       <c r="J187" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
@@ -8657,7 +8657,7 @@
         <v>50</v>
       </c>
       <c r="J188" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
@@ -8709,7 +8709,7 @@
         <v>12</v>
       </c>
       <c r="J190" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
@@ -8738,7 +8738,7 @@
         <v>42</v>
       </c>
       <c r="J191" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
@@ -8764,7 +8764,7 @@
         <v>446</v>
       </c>
       <c r="J192" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="K192" t="s">
         <v>588</v>
@@ -8796,7 +8796,7 @@
         <v>12</v>
       </c>
       <c r="J193" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
@@ -8825,7 +8825,7 @@
         <v>12</v>
       </c>
       <c r="J194" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
@@ -8854,7 +8854,7 @@
         <v>42</v>
       </c>
       <c r="J195" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
@@ -8926,7 +8926,7 @@
         <v>12</v>
       </c>
       <c r="J198" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
@@ -8955,7 +8955,7 @@
         <v>35</v>
       </c>
       <c r="J199" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
@@ -9036,7 +9036,7 @@
         <v>31</v>
       </c>
       <c r="J202" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
@@ -9148,7 +9148,7 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>939</v>
+        <v>1015</v>
       </c>
       <c r="B207" t="s">
         <v>474</v>
@@ -9174,7 +9174,7 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B208" t="s">
         <v>476</v>
@@ -9200,10 +9200,10 @@
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B209" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C209" t="s">
         <v>650</v>
@@ -9224,7 +9224,7 @@
         <v>42</v>
       </c>
       <c r="J209" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K209" t="s">
         <v>704</v>
@@ -9232,10 +9232,10 @@
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B210" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C210" t="s">
         <v>650</v>
@@ -9256,7 +9256,7 @@
         <v>42</v>
       </c>
       <c r="J210" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K210" t="s">
         <v>704</v>
@@ -9264,10 +9264,10 @@
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B211" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C211" t="s">
         <v>650</v>
@@ -9288,7 +9288,7 @@
         <v>42</v>
       </c>
       <c r="J211" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K211" t="s">
         <v>704</v>
@@ -9296,7 +9296,7 @@
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B212" t="s">
         <v>482</v>
@@ -9322,7 +9322,7 @@
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B213" t="s">
         <v>484</v>
@@ -9348,7 +9348,7 @@
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B214" t="s">
         <v>487</v>
@@ -9372,12 +9372,12 @@
         <v>22</v>
       </c>
       <c r="J214" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B215" t="s">
         <v>489</v>
@@ -9401,12 +9401,12 @@
         <v>22</v>
       </c>
       <c r="J215" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B216" t="s">
         <v>491</v>
@@ -9430,12 +9430,12 @@
         <v>22</v>
       </c>
       <c r="J216" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B217" t="s">
         <v>494</v>
@@ -9459,12 +9459,12 @@
         <v>22</v>
       </c>
       <c r="J217" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B218" t="s">
         <v>497</v>
@@ -9487,7 +9487,7 @@
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B219" t="s">
         <v>500</v>
@@ -9511,12 +9511,12 @@
         <v>22</v>
       </c>
       <c r="J219" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B220" t="s">
         <v>502</v>
@@ -9542,7 +9542,7 @@
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B221" t="s">
         <v>504</v>
@@ -9566,12 +9566,12 @@
         <v>12</v>
       </c>
       <c r="J221" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B222" t="s">
         <v>506</v>
@@ -9594,7 +9594,7 @@
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B223" t="s">
         <v>508</v>
@@ -9623,7 +9623,7 @@
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B224" t="s">
         <v>511</v>
@@ -9649,7 +9649,7 @@
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B225" t="s">
         <v>513</v>
@@ -9678,7 +9678,7 @@
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B226" t="s">
         <v>516</v>
@@ -9701,7 +9701,7 @@
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B227" t="s">
         <v>519</v>
@@ -9722,12 +9722,12 @@
         <v>7</v>
       </c>
       <c r="J227" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B228" t="s">
         <v>521</v>
@@ -9753,7 +9753,7 @@
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B229" t="s">
         <v>525</v>
@@ -9776,7 +9776,7 @@
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B230" t="s">
         <v>527</v>
@@ -9808,7 +9808,7 @@
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B231" t="s">
         <v>530</v>
@@ -9832,12 +9832,12 @@
         <v>42</v>
       </c>
       <c r="J231" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B232" t="s">
         <v>532</v>
@@ -9861,12 +9861,12 @@
         <v>35</v>
       </c>
       <c r="J232" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B233" t="s">
         <v>534</v>
@@ -9890,7 +9890,7 @@
         <v>42</v>
       </c>
       <c r="J233" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="K233" t="s">
         <v>588</v>
@@ -9898,7 +9898,7 @@
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B234" t="s">
         <v>537</v>
@@ -9924,7 +9924,7 @@
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B235" t="s">
         <v>540</v>
@@ -9948,12 +9948,12 @@
         <v>31</v>
       </c>
       <c r="J235" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B236" t="s">
         <v>542</v>
@@ -9979,7 +9979,7 @@
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B237" t="s">
         <v>545</v>
@@ -10002,10 +10002,10 @@
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B238" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C238" t="s">
         <v>650</v>
@@ -10026,7 +10026,7 @@
         <v>42</v>
       </c>
       <c r="J238" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K238" t="s">
         <v>704</v>
@@ -10034,10 +10034,10 @@
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B239" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C239" t="s">
         <v>650</v>
@@ -10058,7 +10058,7 @@
         <v>42</v>
       </c>
       <c r="J239" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K239" t="s">
         <v>704</v>

</xml_diff>

<commit_message>
Added "Plaude euge Theotocos"
</commit_message>
<xml_diff>
--- a/!List of all pieces.xlsx
+++ b/!List of all pieces.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="1032">
   <si>
     <t>Title</t>
   </si>
@@ -3102,6 +3102,24 @@
   </si>
   <si>
     <t>frottola</t>
+  </si>
+  <si>
+    <t>plaude_euge_theotocos</t>
+  </si>
+  <si>
+    <t>Plaude euge Theotocos</t>
+  </si>
+  <si>
+    <t>Petrus Wilhelmi Grudencz</t>
+  </si>
+  <si>
+    <t>STB, SBB, ATB, ABB</t>
+  </si>
+  <si>
+    <t>Past Extoling, Theotokos</t>
+  </si>
+  <si>
+    <t>acrostic</t>
   </si>
 </sst>
 </file>
@@ -3428,12 +3446,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K241"/>
+  <dimension ref="A1:K242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
+      <selection pane="bottomLeft" activeCell="J167" sqref="J167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8023,39 +8041,36 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>896</v>
+        <v>1026</v>
       </c>
       <c r="B165" t="s">
-        <v>378</v>
+        <v>1027</v>
       </c>
       <c r="C165" t="s">
-        <v>581</v>
+        <v>1028</v>
       </c>
       <c r="D165" t="s">
-        <v>651</v>
-      </c>
-      <c r="E165" t="s">
-        <v>15</v>
+        <v>1029</v>
       </c>
       <c r="F165" t="s">
-        <v>379</v>
+        <v>1030</v>
       </c>
       <c r="H165" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="I165" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="J165" t="s">
-        <v>977</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B166" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C166" t="s">
         <v>581</v>
@@ -8067,7 +8082,7 @@
         <v>15</v>
       </c>
       <c r="F166" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H166" t="s">
         <v>16</v>
@@ -8081,10 +8096,10 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B167" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C167" t="s">
         <v>581</v>
@@ -8096,7 +8111,7 @@
         <v>15</v>
       </c>
       <c r="F167" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H167" t="s">
         <v>16</v>
@@ -8110,57 +8125,57 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B168" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C168" t="s">
-        <v>617</v>
+        <v>581</v>
       </c>
       <c r="D168" t="s">
         <v>651</v>
       </c>
       <c r="E168" t="s">
-        <v>386</v>
+        <v>15</v>
       </c>
       <c r="F168" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H168" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I168" t="s">
         <v>12</v>
       </c>
       <c r="J168" t="s">
-        <v>971</v>
+        <v>977</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>895</v>
+        <v>899</v>
       </c>
       <c r="B169" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C169" t="s">
-        <v>640</v>
+        <v>617</v>
       </c>
       <c r="D169" t="s">
         <v>651</v>
       </c>
       <c r="E169" t="s">
-        <v>187</v>
+        <v>386</v>
       </c>
       <c r="F169" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H169" t="s">
         <v>8</v>
       </c>
       <c r="I169" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="J169" t="s">
         <v>971</v>
@@ -8168,187 +8183,187 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
       <c r="B170" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C170" t="s">
-        <v>610</v>
+        <v>640</v>
       </c>
       <c r="D170" t="s">
-        <v>668</v>
+        <v>651</v>
+      </c>
+      <c r="E170" t="s">
+        <v>187</v>
       </c>
       <c r="F170" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H170" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="I170" t="s">
-        <v>35</v>
+        <v>42</v>
+      </c>
+      <c r="J170" t="s">
+        <v>971</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B171" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C171" t="s">
-        <v>650</v>
+        <v>610</v>
       </c>
       <c r="D171" t="s">
-        <v>669</v>
-      </c>
-      <c r="E171" t="s">
-        <v>26</v>
+        <v>668</v>
       </c>
       <c r="F171" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H171" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="I171" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B172" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C172" t="s">
-        <v>627</v>
+        <v>650</v>
       </c>
       <c r="D172" t="s">
-        <v>716</v>
+        <v>669</v>
       </c>
       <c r="E172" t="s">
-        <v>216</v>
+        <v>26</v>
       </c>
       <c r="F172" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H172" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="I172" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B173" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C173" t="s">
-        <v>613</v>
+        <v>627</v>
       </c>
       <c r="D173" t="s">
-        <v>651</v>
+        <v>716</v>
+      </c>
+      <c r="E173" t="s">
+        <v>216</v>
       </c>
       <c r="F173" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H173" t="s">
         <v>39</v>
       </c>
       <c r="I173" t="s">
-        <v>12</v>
-      </c>
-      <c r="J173" t="s">
-        <v>971</v>
+        <v>35</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B174" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C174" t="s">
-        <v>650</v>
+        <v>613</v>
       </c>
       <c r="D174" t="s">
-        <v>710</v>
-      </c>
-      <c r="E174" t="s">
-        <v>30</v>
+        <v>651</v>
       </c>
       <c r="F174" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H174" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="I174" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="J174" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B175" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C175" t="s">
         <v>650</v>
       </c>
       <c r="D175" t="s">
-        <v>651</v>
+        <v>710</v>
       </c>
       <c r="E175" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="F175" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H175" t="s">
         <v>27</v>
       </c>
       <c r="I175" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J175" t="s">
-        <v>981</v>
+        <v>973</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B176" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C176" t="s">
-        <v>634</v>
+        <v>650</v>
       </c>
       <c r="D176" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
       <c r="E176" t="s">
-        <v>161</v>
+        <v>53</v>
       </c>
       <c r="F176" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H176" t="s">
         <v>27</v>
       </c>
       <c r="I176" t="s">
-        <v>162</v>
+        <v>35</v>
       </c>
       <c r="J176" t="s">
         <v>981</v>
@@ -8356,146 +8371,146 @@
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B177" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C177" t="s">
-        <v>650</v>
+        <v>634</v>
       </c>
       <c r="D177" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E177" t="s">
-        <v>26</v>
+        <v>161</v>
       </c>
       <c r="F177" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H177" t="s">
-        <v>557</v>
+        <v>27</v>
       </c>
       <c r="I177" t="s">
-        <v>12</v>
+        <v>162</v>
+      </c>
+      <c r="J177" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B178" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C178" t="s">
-        <v>626</v>
+        <v>650</v>
       </c>
       <c r="D178" t="s">
-        <v>717</v>
+        <v>661</v>
+      </c>
+      <c r="E178" t="s">
+        <v>26</v>
       </c>
       <c r="F178" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H178" t="s">
-        <v>27</v>
+        <v>557</v>
       </c>
       <c r="I178" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>765</v>
+        <v>908</v>
       </c>
       <c r="B179" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C179" t="s">
-        <v>596</v>
+        <v>626</v>
       </c>
       <c r="D179" t="s">
-        <v>651</v>
-      </c>
-      <c r="E179" t="s">
-        <v>60</v>
+        <v>717</v>
       </c>
       <c r="F179" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H179" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="I179" t="s">
-        <v>42</v>
-      </c>
-      <c r="J179" t="s">
-        <v>971</v>
+        <v>22</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>909</v>
+        <v>765</v>
       </c>
       <c r="B180" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C180" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="D180" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="E180" t="s">
-        <v>411</v>
+        <v>60</v>
       </c>
       <c r="F180" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H180" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="I180" t="s">
-        <v>35</v>
-      </c>
-      <c r="K180" t="s">
-        <v>588</v>
+        <v>42</v>
+      </c>
+      <c r="J180" t="s">
+        <v>971</v>
       </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B181" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C181" t="s">
-        <v>581</v>
+        <v>591</v>
       </c>
       <c r="D181" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="E181" t="s">
-        <v>15</v>
+        <v>411</v>
       </c>
       <c r="F181" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H181" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="I181" t="s">
-        <v>12</v>
-      </c>
-      <c r="J181" t="s">
-        <v>977</v>
+        <v>35</v>
+      </c>
+      <c r="K181" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B182" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C182" t="s">
         <v>581</v>
@@ -8507,7 +8522,7 @@
         <v>15</v>
       </c>
       <c r="F182" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H182" t="s">
         <v>16</v>
@@ -8521,10 +8536,10 @@
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B183" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C183" t="s">
         <v>581</v>
@@ -8536,7 +8551,7 @@
         <v>15</v>
       </c>
       <c r="F183" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H183" t="s">
         <v>16</v>
@@ -8550,10 +8565,10 @@
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B184" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C184" t="s">
         <v>581</v>
@@ -8565,7 +8580,7 @@
         <v>15</v>
       </c>
       <c r="F184" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H184" t="s">
         <v>16</v>
@@ -8579,10 +8594,10 @@
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B185" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C185" t="s">
         <v>581</v>
@@ -8594,7 +8609,7 @@
         <v>15</v>
       </c>
       <c r="F185" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H185" t="s">
         <v>16</v>
@@ -8608,288 +8623,288 @@
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B186" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C186" t="s">
-        <v>603</v>
+        <v>581</v>
       </c>
       <c r="D186" t="s">
-        <v>718</v>
+        <v>651</v>
+      </c>
+      <c r="E186" t="s">
+        <v>15</v>
       </c>
       <c r="F186" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H186" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="I186" t="s">
-        <v>50</v>
+        <v>12</v>
+      </c>
+      <c r="J186" t="s">
+        <v>977</v>
       </c>
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B187" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C187" t="s">
-        <v>578</v>
+        <v>603</v>
       </c>
       <c r="D187" t="s">
-        <v>657</v>
-      </c>
-      <c r="E187" t="s">
-        <v>158</v>
+        <v>718</v>
       </c>
       <c r="F187" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H187" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I187" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B188" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C188" t="s">
-        <v>626</v>
+        <v>578</v>
       </c>
       <c r="D188" t="s">
-        <v>687</v>
+        <v>657</v>
       </c>
       <c r="E188" t="s">
-        <v>428</v>
+        <v>158</v>
       </c>
       <c r="F188" t="s">
-        <v>427</v>
-      </c>
-      <c r="G188" t="s">
-        <v>568</v>
+        <v>425</v>
       </c>
       <c r="H188" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="I188" t="s">
-        <v>22</v>
-      </c>
-      <c r="J188" t="s">
-        <v>981</v>
+        <v>35</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B189" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C189" t="s">
-        <v>611</v>
+        <v>626</v>
       </c>
       <c r="D189" t="s">
-        <v>651</v>
+        <v>687</v>
       </c>
       <c r="E189" t="s">
-        <v>386</v>
+        <v>428</v>
       </c>
       <c r="F189" t="s">
-        <v>430</v>
+        <v>427</v>
+      </c>
+      <c r="G189" t="s">
+        <v>568</v>
       </c>
       <c r="H189" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="I189" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="J189" t="s">
-        <v>971</v>
+        <v>981</v>
       </c>
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B190" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C190" t="s">
-        <v>650</v>
+        <v>611</v>
       </c>
       <c r="D190" t="s">
         <v>651</v>
       </c>
       <c r="E190" t="s">
-        <v>53</v>
+        <v>386</v>
       </c>
       <c r="F190" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H190" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="I190" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J190" t="s">
-        <v>981</v>
+        <v>971</v>
       </c>
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B191" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C191" t="s">
-        <v>615</v>
+        <v>650</v>
       </c>
       <c r="D191" t="s">
-        <v>719</v>
+        <v>651</v>
+      </c>
+      <c r="E191" t="s">
+        <v>53</v>
       </c>
       <c r="F191" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H191" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="I191" t="s">
-        <v>22</v>
+        <v>50</v>
+      </c>
+      <c r="J191" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B192" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C192" t="s">
-        <v>579</v>
+        <v>615</v>
       </c>
       <c r="D192" t="s">
-        <v>651</v>
-      </c>
-      <c r="E192" t="s">
-        <v>437</v>
+        <v>719</v>
       </c>
       <c r="F192" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H192" t="s">
         <v>39</v>
       </c>
       <c r="I192" t="s">
-        <v>12</v>
-      </c>
-      <c r="J192" t="s">
-        <v>976</v>
+        <v>22</v>
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B193" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C193" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
       <c r="D193" t="s">
         <v>651</v>
       </c>
       <c r="E193" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="F193" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="H193" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="I193" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="J193" t="s">
-        <v>981</v>
+        <v>976</v>
       </c>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B194" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C194" t="s">
-        <v>590</v>
+        <v>612</v>
       </c>
       <c r="D194" t="s">
         <v>651</v>
       </c>
+      <c r="E194" t="s">
+        <v>443</v>
+      </c>
       <c r="F194" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="H194" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I194" t="s">
-        <v>446</v>
+        <v>42</v>
       </c>
       <c r="J194" t="s">
         <v>981</v>
       </c>
-      <c r="K194" t="s">
-        <v>588</v>
-      </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B195" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C195" t="s">
-        <v>581</v>
+        <v>590</v>
       </c>
       <c r="D195" t="s">
         <v>651</v>
       </c>
-      <c r="E195" t="s">
-        <v>15</v>
-      </c>
       <c r="F195" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H195" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="I195" t="s">
-        <v>12</v>
+        <v>446</v>
       </c>
       <c r="J195" t="s">
-        <v>977</v>
+        <v>981</v>
+      </c>
+      <c r="K195" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B196" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C196" t="s">
         <v>581</v>
@@ -8901,7 +8916,7 @@
         <v>15</v>
       </c>
       <c r="F196" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H196" t="s">
         <v>16</v>
@@ -8915,178 +8930,181 @@
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B197" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C197" t="s">
-        <v>641</v>
+        <v>581</v>
       </c>
       <c r="D197" t="s">
         <v>651</v>
       </c>
       <c r="E197" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="F197" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H197" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I197" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="J197" t="s">
-        <v>971</v>
+        <v>977</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B198" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C198" t="s">
-        <v>615</v>
+        <v>641</v>
       </c>
       <c r="D198" t="s">
-        <v>662</v>
+        <v>651</v>
+      </c>
+      <c r="E198" t="s">
+        <v>60</v>
       </c>
       <c r="F198" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="H198" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="I198" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="J198" t="s">
+        <v>971</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B199" t="s">
-        <v>438</v>
+        <v>453</v>
       </c>
       <c r="C199" t="s">
-        <v>636</v>
+        <v>615</v>
       </c>
       <c r="D199" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="F199" t="s">
-        <v>439</v>
+        <v>454</v>
       </c>
       <c r="H199" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I199" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="B200" t="s">
-        <v>455</v>
+        <v>438</v>
       </c>
       <c r="C200" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
       <c r="D200" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="F200" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
       <c r="H200" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I200" t="s">
-        <v>12</v>
-      </c>
-      <c r="J200" t="s">
-        <v>971</v>
+        <v>35</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B201" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C201" t="s">
-        <v>580</v>
+        <v>645</v>
       </c>
       <c r="D201" t="s">
-        <v>720</v>
-      </c>
-      <c r="E201" t="s">
-        <v>216</v>
+        <v>651</v>
       </c>
       <c r="F201" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H201" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I201" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="J201" t="s">
-        <v>978</v>
+        <v>971</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B202" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C202" t="s">
-        <v>635</v>
+        <v>580</v>
       </c>
       <c r="D202" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E202" t="s">
-        <v>461</v>
+        <v>216</v>
       </c>
       <c r="F202" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H202" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I202" t="s">
         <v>35</v>
       </c>
+      <c r="J202" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B203" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C203" t="s">
-        <v>621</v>
+        <v>635</v>
       </c>
       <c r="D203" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E203" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="F203" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H203" t="s">
         <v>39</v>
@@ -9097,158 +9115,158 @@
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B204" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C204" t="s">
-        <v>650</v>
+        <v>621</v>
       </c>
       <c r="D204" t="s">
-        <v>651</v>
+        <v>722</v>
       </c>
       <c r="E204" t="s">
-        <v>30</v>
+        <v>464</v>
       </c>
       <c r="F204" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="H204" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="I204" t="s">
-        <v>31</v>
-      </c>
-      <c r="J204" t="s">
-        <v>973</v>
+        <v>35</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B205" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C205" t="s">
-        <v>610</v>
+        <v>650</v>
       </c>
       <c r="D205" t="s">
-        <v>667</v>
+        <v>651</v>
       </c>
       <c r="E205" t="s">
-        <v>469</v>
+        <v>30</v>
       </c>
       <c r="F205" t="s">
-        <v>468</v>
-      </c>
-      <c r="G205" t="s">
-        <v>574</v>
+        <v>466</v>
       </c>
       <c r="H205" t="s">
         <v>27</v>
       </c>
       <c r="I205" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="J205" t="s">
+        <v>973</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B206" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C206" t="s">
-        <v>650</v>
+        <v>610</v>
       </c>
       <c r="D206" t="s">
-        <v>723</v>
+        <v>667</v>
       </c>
       <c r="E206" t="s">
-        <v>142</v>
+        <v>469</v>
       </c>
       <c r="F206" t="s">
-        <v>471</v>
+        <v>468</v>
+      </c>
+      <c r="G206" t="s">
+        <v>574</v>
       </c>
       <c r="H206" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="I206" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B207" t="s">
-        <v>929</v>
+        <v>470</v>
       </c>
       <c r="C207" t="s">
         <v>650</v>
       </c>
       <c r="D207" t="s">
-        <v>699</v>
+        <v>723</v>
       </c>
       <c r="E207" t="s">
-        <v>26</v>
+        <v>142</v>
       </c>
       <c r="F207" t="s">
-        <v>440</v>
+        <v>471</v>
       </c>
       <c r="H207" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="I207" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B208" t="s">
-        <v>472</v>
+        <v>929</v>
       </c>
       <c r="C208" t="s">
         <v>650</v>
       </c>
       <c r="D208" t="s">
-        <v>651</v>
+        <v>699</v>
       </c>
       <c r="E208" t="s">
-        <v>273</v>
+        <v>26</v>
       </c>
       <c r="F208" t="s">
-        <v>473</v>
+        <v>440</v>
       </c>
       <c r="H208" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="I208" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>1014</v>
+        <v>938</v>
       </c>
       <c r="B209" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C209" t="s">
         <v>650</v>
       </c>
       <c r="D209" t="s">
-        <v>663</v>
+        <v>651</v>
       </c>
       <c r="E209" t="s">
         <v>273</v>
       </c>
       <c r="F209" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H209" t="s">
         <v>27</v>
@@ -9259,68 +9277,62 @@
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>939</v>
+        <v>1014</v>
       </c>
       <c r="B210" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C210" t="s">
         <v>650</v>
       </c>
       <c r="D210" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="E210" t="s">
-        <v>478</v>
+        <v>273</v>
       </c>
       <c r="F210" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H210" t="s">
-        <v>559</v>
+        <v>27</v>
       </c>
       <c r="I210" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B211" t="s">
-        <v>1012</v>
+        <v>476</v>
       </c>
       <c r="C211" t="s">
         <v>650</v>
       </c>
       <c r="D211" t="s">
-        <v>44</v>
+        <v>651</v>
       </c>
       <c r="E211" t="s">
-        <v>41</v>
+        <v>478</v>
       </c>
       <c r="F211" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H211" t="s">
-        <v>43</v>
+        <v>559</v>
       </c>
       <c r="I211" t="s">
-        <v>42</v>
-      </c>
-      <c r="J211" t="s">
-        <v>974</v>
-      </c>
-      <c r="K211" t="s">
-        <v>704</v>
+        <v>12</v>
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B212" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C212" t="s">
         <v>650</v>
@@ -9332,7 +9344,7 @@
         <v>41</v>
       </c>
       <c r="F212" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H212" t="s">
         <v>43</v>
@@ -9349,10 +9361,10 @@
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B213" t="s">
-        <v>989</v>
+        <v>1013</v>
       </c>
       <c r="C213" t="s">
         <v>650</v>
@@ -9364,7 +9376,7 @@
         <v>41</v>
       </c>
       <c r="F213" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H213" t="s">
         <v>43</v>
@@ -9381,51 +9393,57 @@
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B214" t="s">
-        <v>482</v>
+        <v>989</v>
       </c>
       <c r="C214" t="s">
-        <v>599</v>
+        <v>650</v>
       </c>
       <c r="D214" t="s">
-        <v>657</v>
+        <v>44</v>
+      </c>
+      <c r="E214" t="s">
+        <v>41</v>
       </c>
       <c r="F214" t="s">
-        <v>483</v>
-      </c>
-      <c r="G214" t="s">
-        <v>565</v>
+        <v>481</v>
       </c>
       <c r="H214" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I214" t="s">
-        <v>35</v>
+        <v>42</v>
+      </c>
+      <c r="J214" t="s">
+        <v>974</v>
+      </c>
+      <c r="K214" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B215" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C215" t="s">
-        <v>633</v>
+        <v>599</v>
       </c>
       <c r="D215" t="s">
-        <v>691</v>
-      </c>
-      <c r="E215" t="s">
-        <v>486</v>
+        <v>657</v>
       </c>
       <c r="F215" t="s">
-        <v>485</v>
+        <v>483</v>
+      </c>
+      <c r="G215" t="s">
+        <v>565</v>
       </c>
       <c r="H215" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="I215" t="s">
         <v>35</v>
@@ -9433,51 +9451,48 @@
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B216" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C216" t="s">
-        <v>644</v>
+        <v>633</v>
       </c>
       <c r="D216" t="s">
-        <v>724</v>
+        <v>691</v>
       </c>
       <c r="E216" t="s">
-        <v>205</v>
+        <v>486</v>
       </c>
       <c r="F216" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="H216" t="s">
-        <v>559</v>
+        <v>57</v>
       </c>
       <c r="I216" t="s">
-        <v>22</v>
-      </c>
-      <c r="J216" t="s">
-        <v>981</v>
+        <v>35</v>
       </c>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B217" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C217" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="D217" t="s">
-        <v>652</v>
+        <v>724</v>
       </c>
       <c r="E217" t="s">
-        <v>134</v>
+        <v>205</v>
       </c>
       <c r="F217" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H217" t="s">
         <v>559</v>
@@ -9491,25 +9506,25 @@
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B218" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C218" t="s">
         <v>650</v>
       </c>
       <c r="D218" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E218" t="s">
-        <v>493</v>
+        <v>134</v>
       </c>
       <c r="F218" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="H218" t="s">
-        <v>23</v>
+        <v>559</v>
       </c>
       <c r="I218" t="s">
         <v>22</v>
@@ -9520,10 +9535,10 @@
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B219" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C219" t="s">
         <v>650</v>
@@ -9532,10 +9547,10 @@
         <v>651</v>
       </c>
       <c r="E219" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F219" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="H219" t="s">
         <v>23</v>
@@ -9549,580 +9564,577 @@
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B220" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C220" t="s">
-        <v>619</v>
+        <v>650</v>
       </c>
       <c r="D220" t="s">
-        <v>725</v>
+        <v>651</v>
+      </c>
+      <c r="E220" t="s">
+        <v>496</v>
       </c>
       <c r="F220" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="H220" t="s">
-        <v>499</v>
+        <v>23</v>
       </c>
       <c r="I220" t="s">
-        <v>199</v>
+        <v>22</v>
+      </c>
+      <c r="J220" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B221" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C221" t="s">
-        <v>650</v>
+        <v>619</v>
       </c>
       <c r="D221" t="s">
-        <v>683</v>
-      </c>
-      <c r="E221" t="s">
-        <v>96</v>
+        <v>725</v>
       </c>
       <c r="F221" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="H221" t="s">
-        <v>23</v>
+        <v>499</v>
       </c>
       <c r="I221" t="s">
-        <v>22</v>
-      </c>
-      <c r="J221" t="s">
-        <v>981</v>
+        <v>199</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B222" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C222" t="s">
-        <v>569</v>
+        <v>650</v>
       </c>
       <c r="D222" t="s">
-        <v>726</v>
+        <v>683</v>
       </c>
       <c r="E222" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="F222" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="H222" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="I222" t="s">
         <v>22</v>
       </c>
+      <c r="J222" t="s">
+        <v>981</v>
+      </c>
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B223" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C223" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="D223" t="s">
-        <v>651</v>
+        <v>726</v>
       </c>
       <c r="E223" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
       <c r="F223" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H223" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="I223" t="s">
-        <v>12</v>
-      </c>
-      <c r="J223" t="s">
-        <v>977</v>
+        <v>22</v>
       </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B224" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C224" t="s">
-        <v>607</v>
+        <v>581</v>
       </c>
       <c r="D224" t="s">
-        <v>727</v>
+        <v>651</v>
+      </c>
+      <c r="E224" t="s">
+        <v>15</v>
       </c>
       <c r="F224" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H224" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="I224" t="s">
-        <v>50</v>
+        <v>12</v>
+      </c>
+      <c r="J224" t="s">
+        <v>977</v>
       </c>
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B225" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C225" t="s">
-        <v>578</v>
+        <v>607</v>
       </c>
       <c r="D225" t="s">
-        <v>728</v>
-      </c>
-      <c r="E225" t="s">
-        <v>510</v>
+        <v>727</v>
       </c>
       <c r="F225" t="s">
-        <v>509</v>
-      </c>
-      <c r="G225" t="s">
-        <v>565</v>
+        <v>507</v>
       </c>
       <c r="H225" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I225" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B226" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C226" t="s">
-        <v>650</v>
+        <v>578</v>
       </c>
       <c r="D226" t="s">
-        <v>652</v>
+        <v>728</v>
       </c>
       <c r="E226" t="s">
-        <v>142</v>
+        <v>510</v>
       </c>
       <c r="F226" t="s">
-        <v>512</v>
+        <v>509</v>
+      </c>
+      <c r="G226" t="s">
+        <v>565</v>
       </c>
       <c r="H226" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="I226" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B227" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C227" t="s">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="D227" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="E227" t="s">
-        <v>515</v>
+        <v>142</v>
       </c>
       <c r="F227" t="s">
-        <v>514</v>
-      </c>
-      <c r="G227" t="s">
-        <v>565</v>
+        <v>512</v>
       </c>
       <c r="H227" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="I227" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B228" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C228" t="s">
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="D228" t="s">
-        <v>651</v>
+        <v>657</v>
+      </c>
+      <c r="E228" t="s">
+        <v>515</v>
       </c>
       <c r="F228" t="s">
-        <v>517</v>
+        <v>514</v>
+      </c>
+      <c r="G228" t="s">
+        <v>565</v>
       </c>
       <c r="H228" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="I228" t="s">
-        <v>518</v>
+        <v>35</v>
       </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B229" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C229" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="D229" t="s">
         <v>651</v>
       </c>
       <c r="F229" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="H229" t="s">
-        <v>228</v>
+        <v>27</v>
       </c>
       <c r="I229" t="s">
-        <v>7</v>
-      </c>
-      <c r="J229" t="s">
-        <v>975</v>
+        <v>518</v>
       </c>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B230" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C230" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D230" t="s">
-        <v>694</v>
-      </c>
-      <c r="E230" t="s">
-        <v>523</v>
+        <v>651</v>
       </c>
       <c r="F230" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H230" t="s">
-        <v>27</v>
+        <v>228</v>
       </c>
       <c r="I230" t="s">
-        <v>524</v>
+        <v>7</v>
+      </c>
+      <c r="J230" t="s">
+        <v>975</v>
       </c>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B231" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="C231" t="s">
-        <v>618</v>
+        <v>650</v>
       </c>
       <c r="D231" t="s">
-        <v>729</v>
+        <v>694</v>
+      </c>
+      <c r="E231" t="s">
+        <v>523</v>
       </c>
       <c r="F231" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="H231" t="s">
-        <v>228</v>
+        <v>27</v>
       </c>
       <c r="I231" t="s">
-        <v>35</v>
+        <v>524</v>
       </c>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B232" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C232" t="s">
-        <v>639</v>
+        <v>618</v>
       </c>
       <c r="D232" t="s">
-        <v>651</v>
-      </c>
-      <c r="E232" t="s">
-        <v>529</v>
+        <v>729</v>
       </c>
       <c r="F232" t="s">
-        <v>528</v>
-      </c>
-      <c r="G232" t="s">
-        <v>564</v>
+        <v>526</v>
       </c>
       <c r="H232" t="s">
-        <v>27</v>
+        <v>228</v>
       </c>
       <c r="I232" t="s">
-        <v>446</v>
-      </c>
-      <c r="K232" t="s">
-        <v>706</v>
+        <v>35</v>
       </c>
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>966</v>
+        <v>961</v>
       </c>
       <c r="B233" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C233" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D233" t="s">
         <v>651</v>
       </c>
       <c r="E233" t="s">
-        <v>6</v>
+        <v>529</v>
       </c>
       <c r="F233" t="s">
-        <v>531</v>
+        <v>528</v>
+      </c>
+      <c r="G233" t="s">
+        <v>564</v>
       </c>
       <c r="H233" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="I233" t="s">
-        <v>42</v>
-      </c>
-      <c r="J233" t="s">
-        <v>971</v>
+        <v>446</v>
+      </c>
+      <c r="K233" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>962</v>
+        <v>966</v>
       </c>
       <c r="B234" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C234" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="D234" t="s">
-        <v>730</v>
+        <v>651</v>
       </c>
       <c r="E234" t="s">
-        <v>486</v>
+        <v>6</v>
       </c>
       <c r="F234" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H234" t="s">
-        <v>562</v>
+        <v>8</v>
       </c>
       <c r="I234" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J234" t="s">
-        <v>981</v>
+        <v>971</v>
       </c>
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B235" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C235" t="s">
-        <v>594</v>
+        <v>650</v>
       </c>
       <c r="D235" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E235" t="s">
-        <v>536</v>
+        <v>486</v>
       </c>
       <c r="F235" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="H235" t="s">
-        <v>27</v>
+        <v>562</v>
       </c>
       <c r="I235" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J235" t="s">
-        <v>984</v>
-      </c>
-      <c r="K235" t="s">
-        <v>588</v>
+        <v>981</v>
       </c>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B236" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C236" t="s">
-        <v>650</v>
+        <v>594</v>
       </c>
       <c r="D236" t="s">
-        <v>710</v>
+        <v>731</v>
       </c>
       <c r="E236" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F236" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="H236" t="s">
         <v>27</v>
       </c>
       <c r="I236" t="s">
-        <v>12</v>
+        <v>42</v>
+      </c>
+      <c r="J236" t="s">
+        <v>984</v>
+      </c>
+      <c r="K236" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B237" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C237" t="s">
         <v>650</v>
       </c>
       <c r="D237" t="s">
-        <v>651</v>
+        <v>710</v>
       </c>
       <c r="E237" t="s">
-        <v>30</v>
+        <v>539</v>
       </c>
       <c r="F237" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="H237" t="s">
         <v>27</v>
       </c>
       <c r="I237" t="s">
-        <v>31</v>
-      </c>
-      <c r="J237" t="s">
-        <v>973</v>
+        <v>12</v>
       </c>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="B238" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C238" t="s">
-        <v>544</v>
+        <v>650</v>
       </c>
       <c r="D238" t="s">
-        <v>667</v>
+        <v>651</v>
       </c>
       <c r="E238" t="s">
-        <v>142</v>
+        <v>30</v>
       </c>
       <c r="F238" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H238" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="I238" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="J238" t="s">
+        <v>973</v>
       </c>
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B239" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C239" t="s">
-        <v>650</v>
+        <v>544</v>
       </c>
       <c r="D239" t="s">
-        <v>651</v>
+        <v>667</v>
+      </c>
+      <c r="E239" t="s">
+        <v>142</v>
       </c>
       <c r="F239" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="H239" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="I239" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B240" t="s">
-        <v>988</v>
+        <v>545</v>
       </c>
       <c r="C240" t="s">
         <v>650</v>
       </c>
       <c r="D240" t="s">
-        <v>44</v>
-      </c>
-      <c r="E240" t="s">
-        <v>41</v>
+        <v>651</v>
       </c>
       <c r="F240" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="H240" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I240" t="s">
-        <v>42</v>
-      </c>
-      <c r="J240" t="s">
-        <v>974</v>
-      </c>
-      <c r="K240" t="s">
-        <v>704</v>
+        <v>12</v>
       </c>
     </row>
     <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B241" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="C241" t="s">
         <v>650</v>
@@ -10134,7 +10146,7 @@
         <v>41</v>
       </c>
       <c r="F241" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H241" t="s">
         <v>43</v>
@@ -10146,6 +10158,38 @@
         <v>974</v>
       </c>
       <c r="K241" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>970</v>
+      </c>
+      <c r="B242" t="s">
+        <v>987</v>
+      </c>
+      <c r="C242" t="s">
+        <v>650</v>
+      </c>
+      <c r="D242" t="s">
+        <v>44</v>
+      </c>
+      <c r="E242" t="s">
+        <v>41</v>
+      </c>
+      <c r="F242" t="s">
+        <v>548</v>
+      </c>
+      <c r="H242" t="s">
+        <v>43</v>
+      </c>
+      <c r="I242" t="s">
+        <v>42</v>
+      </c>
+      <c r="J242" t="s">
+        <v>974</v>
+      </c>
+      <c r="K242" t="s">
         <v>704</v>
       </c>
     </row>

</xml_diff>